<commit_message>
Release after some NST additions
</commit_message>
<xml_diff>
--- a/src/main/webapp/resources/excelTemplates/nst_template.xlsx
+++ b/src/main/webapp/resources/excelTemplates/nst_template.xlsx
@@ -415,27 +415,27 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -748,7 +748,7 @@
   <dimension ref="A1:AD11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -763,113 +763,113 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
-      <c r="O1" s="18"/>
-      <c r="P1" s="18"/>
-      <c r="Q1" s="18"/>
-      <c r="R1" s="18"/>
-      <c r="S1" s="18"/>
-      <c r="T1" s="18"/>
-      <c r="U1" s="18"/>
-      <c r="V1" s="18"/>
-      <c r="W1" s="18"/>
-      <c r="X1" s="18"/>
-      <c r="Y1" s="18"/>
-      <c r="Z1" s="18"/>
-      <c r="AA1" s="18"/>
-      <c r="AB1" s="18"/>
-      <c r="AC1" s="18"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="15"/>
+      <c r="Q1" s="15"/>
+      <c r="R1" s="15"/>
+      <c r="S1" s="15"/>
+      <c r="T1" s="15"/>
+      <c r="U1" s="15"/>
+      <c r="V1" s="15"/>
+      <c r="W1" s="15"/>
+      <c r="X1" s="15"/>
+      <c r="Y1" s="15"/>
+      <c r="Z1" s="15"/>
+      <c r="AA1" s="15"/>
+      <c r="AB1" s="15"/>
+      <c r="AC1" s="15"/>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="14" t="s">
+      <c r="F3" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="14" t="s">
+      <c r="G3" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="14" t="s">
+      <c r="H3" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="19" t="s">
+      <c r="I3" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="19"/>
-      <c r="K3" s="19"/>
-      <c r="L3" s="19"/>
-      <c r="M3" s="19"/>
-      <c r="N3" s="20" t="s">
+      <c r="J3" s="17"/>
+      <c r="K3" s="17"/>
+      <c r="L3" s="17"/>
+      <c r="M3" s="17"/>
+      <c r="N3" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="O3" s="20"/>
-      <c r="P3" s="20"/>
-      <c r="Q3" s="20"/>
-      <c r="R3" s="20"/>
-      <c r="S3" s="21" t="s">
+      <c r="O3" s="18"/>
+      <c r="P3" s="18"/>
+      <c r="Q3" s="18"/>
+      <c r="R3" s="18"/>
+      <c r="S3" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="T3" s="21"/>
-      <c r="U3" s="21"/>
-      <c r="V3" s="21"/>
-      <c r="W3" s="15" t="s">
+      <c r="T3" s="19"/>
+      <c r="U3" s="19"/>
+      <c r="V3" s="19"/>
+      <c r="W3" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="X3" s="15" t="s">
+      <c r="X3" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="Y3" s="15" t="s">
+      <c r="Y3" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="Z3" s="15" t="s">
+      <c r="Z3" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="AA3" s="15" t="s">
+      <c r="AA3" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="AB3" s="15"/>
-      <c r="AC3" s="15"/>
-      <c r="AD3" s="14" t="s">
+      <c r="AB3" s="20"/>
+      <c r="AC3" s="20"/>
+      <c r="AD3" s="16" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:30" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="14"/>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
+      <c r="A4" s="16"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
       <c r="I4" s="1" t="s">
         <v>18</v>
       </c>
@@ -912,10 +912,10 @@
       <c r="V4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="W4" s="15"/>
-      <c r="X4" s="15"/>
-      <c r="Y4" s="15"/>
-      <c r="Z4" s="15"/>
+      <c r="W4" s="20"/>
+      <c r="X4" s="20"/>
+      <c r="Y4" s="20"/>
+      <c r="Z4" s="20"/>
       <c r="AA4" s="4" t="s">
         <v>23</v>
       </c>
@@ -925,7 +925,7 @@
       <c r="AC4" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="AD4" s="14"/>
+      <c r="AD4" s="16"/>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
@@ -1018,15 +1018,15 @@
       </c>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="16"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
+      <c r="B6" s="21"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="21"/>
       <c r="H6" s="9"/>
       <c r="I6" s="13" t="s">
         <v>51</v>
@@ -1086,37 +1086,37 @@
       <c r="AD6" s="9"/>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="16"/>
-      <c r="I7" s="16"/>
-      <c r="J7" s="16"/>
-      <c r="K7" s="16"/>
-      <c r="L7" s="16"/>
-      <c r="M7" s="16"/>
-      <c r="N7" s="16"/>
-      <c r="O7" s="16"/>
-      <c r="P7" s="16"/>
-      <c r="Q7" s="16"/>
-      <c r="R7" s="16"/>
-      <c r="S7" s="16"/>
-      <c r="T7" s="16"/>
-      <c r="U7" s="16"/>
-      <c r="V7" s="16"/>
-      <c r="W7" s="16"/>
-      <c r="X7" s="16" t="e">
+      <c r="B7" s="21"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="21"/>
+      <c r="I7" s="21"/>
+      <c r="J7" s="21"/>
+      <c r="K7" s="21"/>
+      <c r="L7" s="21"/>
+      <c r="M7" s="21"/>
+      <c r="N7" s="21"/>
+      <c r="O7" s="21"/>
+      <c r="P7" s="21"/>
+      <c r="Q7" s="21"/>
+      <c r="R7" s="21"/>
+      <c r="S7" s="21"/>
+      <c r="T7" s="21"/>
+      <c r="U7" s="21"/>
+      <c r="V7" s="21"/>
+      <c r="W7" s="21"/>
+      <c r="X7" s="21" t="e">
         <f>X6+Y6</f>
         <v>#VALUE!</v>
       </c>
-      <c r="Y7" s="16"/>
-      <c r="Z7" s="16"/>
+      <c r="Y7" s="21"/>
+      <c r="Z7" s="21"/>
       <c r="AA7" s="9"/>
       <c r="AB7" s="9"/>
       <c r="AC7" s="9"/>
@@ -1138,6 +1138,7 @@
       </c>
       <c r="F11" s="10"/>
       <c r="G11" s="10">
+        <f>IF(B11="ГМ",3589.8,646.8)</f>
         <v>646.79999999999995</v>
       </c>
       <c r="H11" s="10" t="s">
@@ -1212,6 +1213,11 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="AD3:AD4"/>
+    <mergeCell ref="AA3:AC3"/>
+    <mergeCell ref="A6:G6"/>
+    <mergeCell ref="A7:W7"/>
+    <mergeCell ref="X7:Z7"/>
     <mergeCell ref="A1:AC1"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="B3:B4"/>
@@ -1228,11 +1234,6 @@
     <mergeCell ref="X3:X4"/>
     <mergeCell ref="Y3:Y4"/>
     <mergeCell ref="Z3:Z4"/>
-    <mergeCell ref="AD3:AD4"/>
-    <mergeCell ref="AA3:AC3"/>
-    <mergeCell ref="A6:G6"/>
-    <mergeCell ref="A7:W7"/>
-    <mergeCell ref="X7:Z7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>